<commit_message>
Atualização da descrição inicial e lista de requisitos/casos de uso
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gvs\git\pescapreco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Educação\Christus\2016.1\APIS\Projeto Final\pescapreco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>RE Nº</t>
   </si>
@@ -62,42 +62,27 @@
     <t>Consumidor</t>
   </si>
   <si>
-    <t>Permitir que o consumidor crie sua própria cesta de produtos</t>
-  </si>
-  <si>
     <t>Consultar preços dos produtos da cesta (própria ou do sistema)</t>
   </si>
   <si>
     <t>Disponibilizar histórico e variação dos preços dos produtos da cesta (própria ou do sistema)</t>
   </si>
   <si>
-    <t>Permitir que o consumidor sugira a inclusão ou remoção de produtos na cesta</t>
-  </si>
-  <si>
     <t>Exigir cadastro do consumidor para fazer sugestões no sistema</t>
   </si>
   <si>
     <t>CASOS DE USO</t>
   </si>
   <si>
-    <t>Cadastrar Preços</t>
-  </si>
-  <si>
     <t>Consultar Preços</t>
   </si>
   <si>
-    <t>Manter Produtos</t>
-  </si>
-  <si>
     <t>Manter Pesquisadores</t>
   </si>
   <si>
     <t>Consultar Solicitações dos Consumidores</t>
   </si>
   <si>
-    <t>Criar Cesta</t>
-  </si>
-  <si>
     <t>Consultar Histórico e Variação de Produtos</t>
   </si>
   <si>
@@ -117,6 +102,27 @@
   </si>
   <si>
     <t>Cadastrar Consumidor</t>
+  </si>
+  <si>
+    <t>A pensar:</t>
+  </si>
+  <si>
+    <t>Imaginar uma forma de validar os preços alimentados pelos pesquisadores, de modo a evitar grandes discrepâncias ou eventuais erros de digitação.</t>
+  </si>
+  <si>
+    <t>Registrar Preços</t>
+  </si>
+  <si>
+    <t>Manter Cesta de Produtos</t>
+  </si>
+  <si>
+    <t>Permitir que o consumidor crie sua própria cesta de produtos, podendo incluir ou retirar produtos cujos preços deseja acompanhar.</t>
+  </si>
+  <si>
+    <t>Manter Cesta Personalizada</t>
+  </si>
+  <si>
+    <t>Permitir que o consumidor sugira a inclusão ou remoção de produtos na cesta do sistema</t>
   </si>
 </sst>
 </file>
@@ -160,11 +166,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +478,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -525,7 +534,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,13 +542,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -553,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -561,69 +570,69 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,13 +640,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +659,18 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inclusão da consulta de menor preço da cesta. Modificações no Diagrama de Casos de Uso
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gvs\git\pescapreco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Educação\Christus\2016.1\APIS\Projeto Final\pescapreco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>RE Nº</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Consultar preços dos produtos da cesta (própria ou do sistema)</t>
   </si>
   <si>
-    <t>Disponibilizar histórico e variação dos preços dos produtos da cesta (própria ou do sistema)</t>
-  </si>
-  <si>
     <t>Exigir cadastro do consumidor para fazer sugestões no sistema</t>
   </si>
   <si>
@@ -132,6 +129,18 @@
   </si>
   <si>
     <t>Efetuar Login</t>
+  </si>
+  <si>
+    <t>Disponibilizar histórico e variação dos menores preços encontrados em um período para os produtos da cesta (própria ou do sistema)</t>
+  </si>
+  <si>
+    <t>Consultar o local mais barato onde se pode adquirir um produto ou todos os produtos da cesta na data atual.</t>
+  </si>
+  <si>
+    <t>Permitir montar a cesta incluindo quantidades dos produtos (na versão inicial, apenas uma unidade de cada produto)</t>
+  </si>
+  <si>
+    <t>Consultar Menor Preço de Cesta</t>
   </si>
 </sst>
 </file>
@@ -492,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -550,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -567,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -592,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -601,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -618,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -635,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -643,7 +652,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -652,7 +661,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -660,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -669,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -677,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -686,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -694,7 +703,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -703,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -711,7 +720,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -720,7 +729,7 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,31 +737,48 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
       <c r="E15">
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>27</v>
+    <row r="20" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>